<commit_message>
Matlab -> Python (#1)
DONE
</commit_message>
<xml_diff>
--- a/01 Lap Sim Parameters List REFERENCE.xlsx
+++ b/01 Lap Sim Parameters List REFERENCE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonvo\Desktop\Jopidas\FSAE\Lap Sim\Lap Simp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiera\Documents\apersonal_documents\formula\JoVogelOverhaul\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD897F3-AC69-4545-81AB-2334E639E692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8C726A-41E1-427A-AAC7-4309165D729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E56B2D8F-1F18-49E2-9DCE-CAEBAF78E5B3}"/>
+    <workbookView xWindow="11466" yWindow="-54" windowWidth="23148" windowHeight="12348" activeTab="2" xr2:uid="{E56B2D8F-1F18-49E2-9DCE-CAEBAF78E5B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -837,7 +837,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -880,6 +880,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -1292,7 +1298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1375,6 +1381,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1420,27 +1447,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1456,18 +1462,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1803,16 +1833,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
@@ -1841,7 +1871,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="49" t="s">
         <v>103</v>
       </c>
       <c r="B3" s="27" t="s">
@@ -1865,7 +1895,7 @@
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="43"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="28" t="s">
         <v>10</v>
       </c>
@@ -1889,7 +1919,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="29" t="s">
         <v>13</v>
       </c>
@@ -1913,7 +1943,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -1937,7 +1967,7 @@
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="28" t="s">
         <v>24</v>
       </c>
@@ -1961,7 +1991,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="28" t="s">
         <v>28</v>
       </c>
@@ -1985,7 +2015,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="28" t="s">
         <v>31</v>
       </c>
@@ -2009,7 +2039,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="28" t="s">
         <v>38</v>
       </c>
@@ -2033,7 +2063,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="28" t="s">
         <v>41</v>
       </c>
@@ -2055,7 +2085,7 @@
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="50"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="29" t="s">
         <v>44</v>
       </c>
@@ -2079,7 +2109,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="58" t="s">
         <v>106</v>
       </c>
       <c r="B13" s="27" t="s">
@@ -2105,7 +2135,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="28" t="s">
         <v>50</v>
       </c>
@@ -2127,7 +2157,7 @@
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="28" t="s">
         <v>53</v>
       </c>
@@ -2149,7 +2179,7 @@
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="28" t="s">
         <v>55</v>
       </c>
@@ -2171,7 +2201,7 @@
       <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="28" t="s">
         <v>57</v>
       </c>
@@ -2193,7 +2223,7 @@
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="28" t="s">
         <v>59</v>
       </c>
@@ -2215,7 +2245,7 @@
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="53"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="29" t="s">
         <v>60</v>
       </c>
@@ -2237,7 +2267,7 @@
       <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="61" t="s">
         <v>107</v>
       </c>
       <c r="B20" s="27" t="s">
@@ -2258,12 +2288,12 @@
       <c r="G20" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="60" t="s">
+      <c r="H20" s="45" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="28" t="s">
         <v>67</v>
       </c>
@@ -2282,10 +2312,10 @@
       <c r="G21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H21" s="61"/>
+      <c r="H21" s="46"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="55"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="28" t="s">
         <v>69</v>
       </c>
@@ -2304,10 +2334,10 @@
       <c r="G22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H22" s="61"/>
+      <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="28" t="s">
         <v>71</v>
       </c>
@@ -2326,12 +2356,12 @@
       <c r="G23" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="62" t="s">
+      <c r="H23" s="47" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="55"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="28" t="s">
         <v>75</v>
       </c>
@@ -2350,10 +2380,10 @@
       <c r="G24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="62"/>
+      <c r="H24" s="47"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="28" t="s">
         <v>77</v>
       </c>
@@ -2372,12 +2402,12 @@
       <c r="G25" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="62" t="s">
+      <c r="H25" s="47" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="55"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="28" t="s">
         <v>79</v>
       </c>
@@ -2396,10 +2426,10 @@
       <c r="G26" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="62"/>
+      <c r="H26" s="47"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="55"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="28" t="s">
         <v>83</v>
       </c>
@@ -2418,12 +2448,12 @@
       <c r="G27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="62" t="s">
+      <c r="H27" s="47" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="55"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="28" t="s">
         <v>86</v>
       </c>
@@ -2442,10 +2472,10 @@
       <c r="G28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H28" s="62"/>
+      <c r="H28" s="47"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="55"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="28" t="s">
         <v>88</v>
       </c>
@@ -2464,12 +2494,12 @@
       <c r="G29" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="62" t="s">
+      <c r="H29" s="47" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="55"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="28" t="s">
         <v>92</v>
       </c>
@@ -2488,10 +2518,10 @@
       <c r="G30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="62"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="55"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="28" t="s">
         <v>94</v>
       </c>
@@ -2510,12 +2540,12 @@
       <c r="G31" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H31" s="62" t="s">
+      <c r="H31" s="47" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
+      <c r="A32" s="63"/>
       <c r="B32" s="29" t="s">
         <v>95</v>
       </c>
@@ -2534,10 +2564,10 @@
       <c r="G32" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="63"/>
+      <c r="H32" s="48"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="42" t="s">
         <v>108</v>
       </c>
       <c r="B33" s="27" t="s">
@@ -2561,7 +2591,7 @@
       <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="58"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="28" t="s">
         <v>110</v>
       </c>
@@ -2583,7 +2613,7 @@
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="59"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="29" t="s">
         <v>111</v>
       </c>
@@ -2608,6 +2638,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="H20:H22"/>
     <mergeCell ref="H23:H24"/>
@@ -2615,11 +2650,6 @@
     <mergeCell ref="H27:H28"/>
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="H31:H32"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3173,7 +3203,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3185,12 +3215,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="34" t="s">
@@ -3221,19 +3251,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72" t="s">
+      <c r="A4" s="69"/>
+      <c r="B4" s="84" t="s">
         <v>239</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="85" t="s">
         <v>208</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="86" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="69"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="7" t="s">
         <v>200</v>
       </c>
@@ -3245,7 +3275,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="69"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="7" t="s">
         <v>201</v>
       </c>
@@ -3257,7 +3287,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="69"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="7" t="s">
         <v>202</v>
       </c>
@@ -3269,7 +3299,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="70"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="13" t="s">
         <v>203</v>
       </c>
@@ -3281,64 +3311,64 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="75" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="76"/>
+      <c r="B10" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="78" t="s">
         <v>209</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="79" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="76"/>
+      <c r="B11" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="78" t="s">
         <v>209</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="79" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="76"/>
+      <c r="B12" s="77" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="78" t="s">
         <v>209</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="79" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="70"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="80"/>
+      <c r="B13" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="83" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3371,7 +3401,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="70"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="13" t="s">
         <v>205</v>
       </c>
@@ -3397,7 +3427,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="69"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="7" t="s">
         <v>207</v>
       </c>
@@ -3409,7 +3439,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="69"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="7" t="s">
         <v>210</v>
       </c>
@@ -3421,7 +3451,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="69"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="7" t="s">
         <v>211</v>
       </c>
@@ -3433,7 +3463,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="69"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="7" t="s">
         <v>237</v>
       </c>
@@ -3445,7 +3475,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="69"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="7" t="s">
         <v>212</v>
       </c>
@@ -3457,7 +3487,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="70"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="13" t="s">
         <v>213</v>
       </c>

</xml_diff>